<commit_message>
fix group assignment in phylo tree
</commit_message>
<xml_diff>
--- a/STORE_model/notebooks/phylodata/phyloDist.xlsx
+++ b/STORE_model/notebooks/phylodata/phyloDist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\STORE_model\notebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\STORE_model\notebooks\phylodata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43FDECD-6EEE-4A4B-ABBC-8CDF8ADA14C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AE0E92-86DC-4DB6-93B8-63203B06C67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{29FE2FE4-60CD-4039-936F-DD491A058D5F}"/>
+    <workbookView xWindow="4920" yWindow="9885" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{29FE2FE4-60CD-4039-936F-DD491A058D5F}"/>
   </bookViews>
   <sheets>
     <sheet name="phyloDist" sheetId="1" r:id="rId1"/>
@@ -47631,8 +47631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F716B9-87C3-4640-9F47-C1031AAB6F45}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47743,7 +47743,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
         <v>80</v>
@@ -47757,7 +47757,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
         <v>74</v>

</xml_diff>